<commit_message>
Admin1 upadted pom classes
</commit_message>
<xml_diff>
--- a/GUISeleniumFramework/testdata/testScriptdata.xlsx
+++ b/GUISeleniumFramework/testdata/testScriptdata.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B66EEE0E-7793-4D98-9BEE-A78371A6E345}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\GUIFramework\GUISeleniumFramework\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11620" windowHeight="6330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11625" windowHeight="6330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="3" r:id="rId1"/>
-    <sheet name="org" sheetId="1" r:id="rId2"/>
-    <sheet name="product" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="Admin1" sheetId="5" r:id="rId2"/>
+    <sheet name="org" sheetId="1" r:id="rId3"/>
+    <sheet name="product" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="161">
   <si>
     <t>TC_ID</t>
   </si>
@@ -444,13 +448,76 @@
   </si>
   <si>
     <t>faceBook_kdd</t>
+  </si>
+  <si>
+    <t>DoctorName</t>
+  </si>
+  <si>
+    <t>DoctorSpecialization</t>
+  </si>
+  <si>
+    <t>Dermatologists</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>fees</t>
+  </si>
+  <si>
+    <t>phone no</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>confirm password</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>Add_Doctor</t>
+  </si>
+  <si>
+    <t>Chandan</t>
+  </si>
+  <si>
+    <t>2nd cross,vijaynagar,Mandya</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>9585985585</t>
+  </si>
+  <si>
+    <t>chandu@gmail.com</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>edit_Doctor</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>8594259874</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,8 +525,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF5B5B60"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,8 +553,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -507,19 +594,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFE2E2E4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -797,22 +900,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618505B5-BC18-40DF-B31F-D9D1863412AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,7 +930,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>115</v>
       </c>
@@ -840,14 +943,14 @@
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,7 +965,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>116</v>
       </c>
@@ -875,14 +978,14 @@
       <c r="D5" s="3"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -899,7 +1002,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>127</v>
       </c>
@@ -920,21 +1023,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -942,160 +1049,214 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>141</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6E95A9-5958-495C-AC30-1DA708189BFF}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>135</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>138</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1103,20 +1264,71 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7004AA42-F8FF-45C9-AB36-1F51EDB304F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1124,7 +1336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1132,7 +1344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1140,7 +1352,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1148,7 +1360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1156,7 +1368,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1164,7 +1376,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1172,7 +1384,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1180,7 +1392,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1188,7 +1400,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1196,7 +1408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1204,7 +1416,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1212,7 +1424,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1220,7 +1432,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1228,7 +1440,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1236,7 +1448,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1244,7 +1456,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1252,7 +1464,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1260,7 +1472,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1268,7 +1480,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1276,7 +1488,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1284,7 +1496,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1292,7 +1504,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1300,7 +1512,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -1308,7 +1520,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -1316,7 +1528,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -1324,7 +1536,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
@@ -1332,7 +1544,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -1340,7 +1552,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1348,7 +1560,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
@@ -1356,7 +1568,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -1364,7 +1576,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -1372,7 +1584,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -1380,7 +1592,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
@@ -1388,7 +1600,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
@@ -1396,7 +1608,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -1404,7 +1616,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
@@ -1412,7 +1624,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
@@ -1420,7 +1632,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>14</v>
       </c>
@@ -1428,7 +1640,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
@@ -1436,7 +1648,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>14</v>
       </c>
@@ -1444,7 +1656,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +1664,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
@@ -1460,7 +1672,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>14</v>
       </c>
@@ -1468,7 +1680,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>14</v>
       </c>
@@ -1476,7 +1688,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -1484,7 +1696,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>14</v>
       </c>
@@ -1492,7 +1704,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>14</v>
       </c>
@@ -1500,7 +1712,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
@@ -1508,7 +1720,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>14</v>
       </c>
@@ -1516,7 +1728,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>58</v>
       </c>
@@ -1524,7 +1736,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>58</v>
       </c>
@@ -1532,7 +1744,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>58</v>
       </c>
@@ -1540,7 +1752,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>58</v>
       </c>
@@ -1548,7 +1760,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>58</v>
       </c>
@@ -1556,7 +1768,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>58</v>
       </c>
@@ -1564,7 +1776,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>58</v>
       </c>
@@ -1572,7 +1784,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>58</v>
       </c>
@@ -1580,7 +1792,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>58</v>
       </c>
@@ -1588,7 +1800,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>58</v>
       </c>
@@ -1596,7 +1808,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
@@ -1604,7 +1816,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>58</v>
       </c>
@@ -1612,7 +1824,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>58</v>
       </c>
@@ -1620,7 +1832,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>58</v>
       </c>
@@ -1628,7 +1840,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>58</v>
       </c>
@@ -1636,7 +1848,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>58</v>
       </c>
@@ -1644,7 +1856,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>58</v>
       </c>
@@ -1652,7 +1864,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>58</v>
       </c>
@@ -1660,7 +1872,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>58</v>
       </c>
@@ -1668,7 +1880,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>58</v>
       </c>
@@ -1676,7 +1888,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>58</v>
       </c>
@@ -1684,7 +1896,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>58</v>
       </c>
@@ -1692,7 +1904,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>58</v>
       </c>
@@ -1700,7 +1912,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>58</v>
       </c>
@@ -1708,7 +1920,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>58</v>
       </c>
@@ -1716,7 +1928,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>58</v>
       </c>
@@ -1724,7 +1936,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>58</v>
       </c>
@@ -1732,7 +1944,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>58</v>
       </c>
@@ -1740,7 +1952,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>58</v>
       </c>
@@ -1748,7 +1960,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>58</v>
       </c>
@@ -1756,7 +1968,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>58</v>
       </c>
@@ -1764,7 +1976,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>58</v>
       </c>
@@ -1772,7 +1984,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>58</v>
       </c>
@@ -1780,7 +1992,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>58</v>
       </c>
@@ -1788,7 +2000,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>58</v>
       </c>
@@ -1796,7 +2008,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>58</v>
       </c>
@@ -1804,7 +2016,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>58</v>
       </c>
@@ -1812,7 +2024,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>58</v>
       </c>
@@ -1820,7 +2032,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>58</v>
       </c>
@@ -1828,7 +2040,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>58</v>
       </c>
@@ -1836,7 +2048,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>58</v>
       </c>
@@ -1844,7 +2056,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>58</v>
       </c>
@@ -1852,7 +2064,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>58</v>
       </c>
@@ -1860,7 +2072,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>58</v>
       </c>
@@ -1868,7 +2080,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>58</v>
       </c>
@@ -1876,7 +2088,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>58</v>
       </c>
@@ -1884,7 +2096,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>58</v>
       </c>
@@ -1892,7 +2104,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>58</v>
       </c>
@@ -1900,7 +2112,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>58</v>
       </c>
@@ -1908,7 +2120,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>58</v>
       </c>

</xml_diff>